<commit_message>
update: hands on tips
</commit_message>
<xml_diff>
--- a/replying_example.xlsx
+++ b/replying_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linchunho/Developer/aws-line-business-card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DD8498-BC54-BC49-8B6D-8B6B3D7B5B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A39A6E-2FA1-2748-9F8F-8D5DB8946C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{D55B5DE5-8CC8-FA43-A44A-1EC28E00D7B0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D55B5DE5-8CC8-FA43-A44A-1EC28E00D7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>LINE BOT 關鍵字</t>
   </si>
@@ -143,6 +143,21 @@
   </si>
   <si>
     <t>我想了解 AWS LINE BOT 開發團隊 4</t>
+  </si>
+  <si>
+    <t>設定加入好友訊息</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HiHi </t>
+  </si>
+  <si>
+    <t>HiHiHi</t>
+  </si>
+  <si>
+    <t>HiHiHiHi</t>
   </si>
 </sst>
 </file>
@@ -500,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEED68EE-8F55-6B45-9B4F-290EFB89BAB9}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,103 +550,120 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>